<commit_message>
update score report file FR
</commit_message>
<xml_diff>
--- a/export/Outil d'évaluation des coûts du RSI - Rapport de score vierge.xlsx
+++ b/export/Outil d'évaluation des coûts du RSI - Rapport de score vierge.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="48720" yWindow="5880" windowWidth="28800" windowHeight="11080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="1" r:id="rId1"/>
@@ -21,207 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
   <si>
-    <t>P.3.1 Antimicrobial resistance (AMR) detection</t>
-  </si>
-  <si>
-    <t>P.3.2 Surveillance of infections caused by AMR pathogens</t>
-  </si>
-  <si>
-    <t>P.3.4 Antimicrobial stewardship activities</t>
-  </si>
-  <si>
-    <t>Biosafety and Biosecurity</t>
-  </si>
-  <si>
-    <t>Chemical Events</t>
-  </si>
-  <si>
-    <t>Emergency Response Operations</t>
-  </si>
-  <si>
-    <t>R.2.1 Capacity to Activate Emergency Operations</t>
-  </si>
-  <si>
-    <t>R.2.3 Emergency Operations Program</t>
-  </si>
-  <si>
-    <t>R.2.4 Case management procedures are implemented for IHR relevant hazards</t>
-  </si>
-  <si>
-    <t>Food Safety</t>
-  </si>
-  <si>
-    <t>IHR Coordination, Communication and Advocacy</t>
-  </si>
-  <si>
-    <t>Immunization</t>
-  </si>
-  <si>
-    <t>P.7.1 Vaccine coverage (measles) as part of national program</t>
-  </si>
-  <si>
-    <t>P.7.2 National vaccine access and delivery</t>
-  </si>
-  <si>
-    <t>Linking Public Health and Security Authorities</t>
-  </si>
-  <si>
-    <t>R.3.1 Public Health and Security Authorities, (e.g. Law Enforcement, Border Control, Customs) are linked during a suspect or confirmed biological event</t>
-  </si>
-  <si>
-    <t>Medical Countermeasures and Personnel Deployment</t>
-  </si>
-  <si>
-    <t>R.4.1 System is in place for sending and receiving medical countermeasures during a public health emergency</t>
-  </si>
-  <si>
-    <t>R.4.2 System is in place for sending and receiving health personnel during a public health emergency</t>
-  </si>
-  <si>
-    <t>National Laboratory System</t>
-  </si>
-  <si>
-    <t>D.1.1 Laboratory testing for detection of priority diseases</t>
-  </si>
-  <si>
-    <t>D.1.2 Specimen referral and transport system</t>
-  </si>
-  <si>
-    <t>D.1.4 Laboratory Quality System</t>
-  </si>
-  <si>
-    <t>Points of Entry (PoE)</t>
-  </si>
-  <si>
-    <t>Preparedness</t>
-  </si>
-  <si>
-    <t>RE.2 Enabling environment is in place for management of Radiation Emergencies</t>
-  </si>
-  <si>
-    <t>D.2.1 Indicator and event based surveillance systems</t>
-  </si>
-  <si>
-    <t>D.2.4 Syndromic surveillance systems</t>
-  </si>
-  <si>
-    <t>Reporting</t>
-  </si>
-  <si>
-    <t>D.3.2 Reporting network and protocols in country</t>
-  </si>
-  <si>
-    <t>Risk Communication</t>
-  </si>
-  <si>
-    <t>R.5.2 Internal and Partner Communication and Coordination</t>
-  </si>
-  <si>
-    <t>R.5.3 Public Communication</t>
-  </si>
-  <si>
-    <t>R.5.4 Communication Engagement with Affected Communities</t>
-  </si>
-  <si>
-    <t>Workforce Development</t>
-  </si>
-  <si>
-    <t>D.4.1 Human resources are available to implement IHR core capacity requirements</t>
-  </si>
-  <si>
-    <t>D.4.3 Workforce strategy</t>
-  </si>
-  <si>
-    <t>Zoonotic Disease</t>
-  </si>
-  <si>
-    <t>P.4.1 Surveillance systems in place for priority zoonotic diseases/pathogens</t>
-  </si>
-  <si>
-    <t>P.4.2 Veterinary or Animal Health Workforce</t>
-  </si>
-  <si>
-    <t>D.1.3 Effective modern point of care and laboratory based diagnostics</t>
-  </si>
-  <si>
-    <t>National Legislation, Policy, and Financing</t>
-  </si>
-  <si>
-    <t>P.1.1 Legislation, laws, regulations, administrative requirements, policies or other government instruments in place are sufficient for implementation of IHR.</t>
-  </si>
-  <si>
-    <t>P.1.2 The state can demonstrate that it has adjusted and aligned its domestic legislation, policies, and administrative arrangements to enable compliance with the IHR (2005).</t>
-  </si>
-  <si>
-    <t>P.2.1 A functional mechanism is established for the coordination and integration of relevant sectors in the implementation of IHR</t>
-  </si>
-  <si>
-    <t>Antimicrobial Resistance (AMR)</t>
-  </si>
-  <si>
-    <t>P.3.3 Healthcare associated infection (HCAI) prevention control programs</t>
-  </si>
-  <si>
-    <t>P.4.3 Mechanisms for responding to infectious zoonoses and potential zoonoses are established and functional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P.5.1 Mechanisms are established and functioning for detecting and responding to foodborne disease and food contamination. </t>
-  </si>
-  <si>
-    <t>P.6.1 Whole-of-government biosafety and biosecurity system is in place for human, animal, and agriculture facilities</t>
-  </si>
-  <si>
-    <t>P.6.2 Biosafety and biosecurity training practices</t>
-  </si>
-  <si>
-    <t>Real Time Surveillance</t>
-  </si>
-  <si>
-    <t>D.2.2 Interoperable, interconnected, electronic real-time reporting system</t>
-  </si>
-  <si>
-    <t>D.2.3 Integration and analysis of surveillance data</t>
-  </si>
-  <si>
-    <t>D.3.1 System for efficient reporting to WHO, FAO and OIE</t>
-  </si>
-  <si>
-    <t>D.4.2 Applied epidemiology training program in place such as FETP</t>
-  </si>
-  <si>
-    <t>R.1.1 Multi-hazard national public health emergency preparedness and response plan is developed and implemented</t>
-  </si>
-  <si>
-    <t>R.1.2  Priority public health risks and resources are mapped and utilized</t>
-  </si>
-  <si>
-    <t>R.2.2 Emergency Operations Centre Operating Procedures and Plan</t>
-  </si>
-  <si>
-    <t>R.5.1 Risk Communication Systems (plans,mechanisms, etc.)</t>
-  </si>
-  <si>
-    <t>R.5.5 Dynamic Listening and Rumour Management</t>
-  </si>
-  <si>
-    <t>PoE.1 Routine capacities are established at PoE</t>
-  </si>
-  <si>
-    <t>PoE.2 Effective Public Health Response at Points of Entry</t>
-  </si>
-  <si>
-    <t>CE.1 Mechanisms are established and functioning for detecting and responding to chemical events or emergencies</t>
-  </si>
-  <si>
-    <t>CE.2 Enabling environment is in place for management of chemical event</t>
-  </si>
-  <si>
-    <t>Radiological Events</t>
-  </si>
-  <si>
-    <t>RE.1 Mechanisms are established and functioning for detecting and responding to radiological and nuclear emergencies</t>
-  </si>
-  <si>
     <t>Pays</t>
   </si>
   <si>
@@ -231,7 +30,210 @@
     <t>Indicateurs</t>
   </si>
   <si>
-    <t>Cibles (1 à 5)</t>
+    <t>Scores (1 à 5)</t>
+  </si>
+  <si>
+    <t>Législation nationale, réglementation et financement</t>
+  </si>
+  <si>
+    <t>P.1.1 La législation, les lois, les règlements, les exigences administratives, les politiques ou autres instruments gouvernementaux en place suffisent à la mise en œuvre du RSI.</t>
+  </si>
+  <si>
+    <t>P.1.2 L'État peut démontrer qu'il a amendé et aligné sa législation, ses politiques et ses dispositions administratives internes pour permettre la conformité avec le RSI (2005).</t>
+  </si>
+  <si>
+    <t>Coordination, communication et plaidoyer en matière de RSI</t>
+  </si>
+  <si>
+    <t>P.2.1 Un mécanisme fonctionnel est établi pour la coordination et l'intégration des secteurs concernés dans la mise en œuvre du RSI</t>
+  </si>
+  <si>
+    <t>Résistance antimicrobienne (RAM)</t>
+  </si>
+  <si>
+    <t>P.3.1 Détection de la résistance aux antimicrobiens (RAM)</t>
+  </si>
+  <si>
+    <t>P.3.2 Surveillance des infections causées par des agents pathogènes de la RAM</t>
+  </si>
+  <si>
+    <t>P.3.3 Programmes de contrôle de la prévention des infections nosocomiales</t>
+  </si>
+  <si>
+    <t>P.3.4 Activités de gérance des antimicrobiens</t>
+  </si>
+  <si>
+    <t>Maladie zoonotique (zoonose)</t>
+  </si>
+  <si>
+    <t>P.4.1 Systèmes de surveillance en place pour les maladies / agents pathogènes zoonotiques prioritaires</t>
+  </si>
+  <si>
+    <t>P.4.2 Personnel de santé vétérinaire ou animale</t>
+  </si>
+  <si>
+    <t>P.4.3 Les mécanismes d'intervention aux zoonoses infectieuses et aux zoonoses potentielles sont établis et fonctionnels</t>
+  </si>
+  <si>
+    <t>La sécurité alimentaire</t>
+  </si>
+  <si>
+    <t>P.5.1 Des mécanismes sont établis et fonctionnent pour détecter et intervenir face aux maladies d'origine alimentaire et à la contamination des aliments.</t>
+  </si>
+  <si>
+    <t>Biosécurité et biosûreté</t>
+  </si>
+  <si>
+    <t>P.6.1 Un système de biosécurité et de biosûreté pangouvernemental est en place pour les installations humaines, animales et agricoles</t>
+  </si>
+  <si>
+    <t>P.6.2 Pratiques de formation en biosécurité et biosûreté</t>
+  </si>
+  <si>
+    <t>Vaccination</t>
+  </si>
+  <si>
+    <t>P.7.1 Couverture vaccinale (rougeole) dans le cadre du programme national</t>
+  </si>
+  <si>
+    <t>P.7.2 Accès et livraison de vaccins à l'échelle nationale</t>
+  </si>
+  <si>
+    <t>Système de laboratoire national</t>
+  </si>
+  <si>
+    <t>D.1.1 Essais de laboratoire pour la détection de maladies prioritaires</t>
+  </si>
+  <si>
+    <t>D.1.2 Système de référence pour le transfert et le transport d’échantillons</t>
+  </si>
+  <si>
+    <t>D.1.3 Point de soin moderne efficace et diagnostic en laboratoire</t>
+  </si>
+  <si>
+    <t>D.1.4 Système de contrôle-qualité de laboratoire</t>
+  </si>
+  <si>
+    <t>Surveillance en temps réel</t>
+  </si>
+  <si>
+    <t>D.2.1 Systèmes de surveillance fondés sur des indicateurs et des événements</t>
+  </si>
+  <si>
+    <t>D.2.2 Système interopérable, interconnecté, de notification électronique en temps réel</t>
+  </si>
+  <si>
+    <t>D.2.3 Intégration et analyse des données de surveillance</t>
+  </si>
+  <si>
+    <t>D.2.4 Systèmes de surveillance syndromique</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>D.3.1 Système de notification efficace à l'OMS, à la FAO et à l'OIE</t>
+  </si>
+  <si>
+    <t>D.3.2 Réseau de notification et de protocoles dans le pays</t>
+  </si>
+  <si>
+    <t>Développement des ressources humaines</t>
+  </si>
+  <si>
+    <t>D.4.1 Des ressources humaines sont disponibles pour mettre en œuvre les exigences de capacité de base du RSI</t>
+  </si>
+  <si>
+    <t>D.4.2 Programme de formation en épidémiologie appliquée tel que le Programme de Formation en Epidémiologie de Terrain (FETP en Anglais)</t>
+  </si>
+  <si>
+    <t>D.4.3 Stratégie de ressources humaines</t>
+  </si>
+  <si>
+    <t>Préparation</t>
+  </si>
+  <si>
+    <t>R.1.1 Un plan national de préparation et d'intervention en cas d'urgence sanitaire multirisque est élaboré et mis en œuvre</t>
+  </si>
+  <si>
+    <t>R.1.2 Les risques et les ressources prioritaires en matière de santé publique sont cartographiés et utilisés</t>
+  </si>
+  <si>
+    <t>Opérations d'intervention d'urgence</t>
+  </si>
+  <si>
+    <t>R.2.1 Capacité d'activer les interventions d'urgence</t>
+  </si>
+  <si>
+    <t>R.2.2 Procédures et plan opérationel du Centre des Opérations d'Urgence</t>
+  </si>
+  <si>
+    <t>R.2.3 Programme d'interventions d'urgence</t>
+  </si>
+  <si>
+    <t>R.2.4 Des procédures de prise en charge de cas sont mises en œuvre pour les dangers relevant au RSI</t>
+  </si>
+  <si>
+    <t>Lier les autorités de santé publique et les autorités de sécurité</t>
+  </si>
+  <si>
+    <t>R.3.1 Les autorités chargées de la santé publique et de la sécurité (par exemple, l'application de la loi, le contrôle des frontières, les douanes) sont en liaison lors d'un événement biologique suspect ou confirmé</t>
+  </si>
+  <si>
+    <t>Contre-mesures médicales et déploiement du personnel</t>
+  </si>
+  <si>
+    <t>R.4.1 Le système est en place pour l'envois et la réception de moyens médicaux lors d'une urgence de santé publique</t>
+  </si>
+  <si>
+    <t>R.4.2 Le système est en place pour l'envois et la réception de personnels de santé pendant une urgence de santé publique</t>
+  </si>
+  <si>
+    <t>Communication sur les risques</t>
+  </si>
+  <si>
+    <t>R.5.1 Systèmes de communication des risques (plans, mécanismes, etc.)</t>
+  </si>
+  <si>
+    <t>R.5.2 Communication et coordination internes et avec les partenaires</t>
+  </si>
+  <si>
+    <t>R.5.3 Communication publique</t>
+  </si>
+  <si>
+    <t>R.5.4 Communication pour faire participer les communautés touchées</t>
+  </si>
+  <si>
+    <t>R.5.5 Écoute dynamique et gestion des rumeurs</t>
+  </si>
+  <si>
+    <t>Points d'entrée (PdE)</t>
+  </si>
+  <si>
+    <t>POE.1 Les capacités de routine sont établies aux points d'entrée</t>
+  </si>
+  <si>
+    <t>POE.2 Intervention efficace en santé publique aux points d'entrée</t>
+  </si>
+  <si>
+    <t>Événements chimiques</t>
+  </si>
+  <si>
+    <t>CE.1 Mécanismes fonctionnels en place pour la détection et la riposte à des événements/urgences
+d’origine chimique</t>
+  </si>
+  <si>
+    <t>CE.2 Un environnement favorable est en place pour la gestion des événements chimiques</t>
+  </si>
+  <si>
+    <t>Urgences radiologiques</t>
+  </si>
+  <si>
+    <t>RE.1 Mécanismes fonctionnels en place pour la détection et la riposte aux situations
+d’urgence radiologique et nucléaire.</t>
+  </si>
+  <si>
+    <t>RE.2 Un environnement favorable est en place pour la gestion des urgences radiologiques</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1114,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1125,400 +1127,400 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="C46" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>